<commit_message>
updated script and added boxplots
</commit_message>
<xml_diff>
--- a/experiment/datasets/results.xlsx
+++ b/experiment/datasets/results.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oroncal/workspace/research/intino/replication-package/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oroncal/workspace/research/intino/experiment/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09478AC9-905C-FB4A-A89E-E6F3E166B2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E895B734-2157-054D-A30F-0942C24F82CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1320" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{3CBF39F1-3B9A-8146-8AAD-FEF7773C7A1D}"/>
+    <workbookView xWindow="1460" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{3CBF39F1-3B9A-8146-8AAD-FEF7773C7A1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Questionary" sheetId="2" r:id="rId1"/>
+    <sheet name="Task" sheetId="1" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$A$1:$E$1</definedName>
-    <definedName name="Intino_Usability_Study__respuestas____Respuestas_de_formulario_1" localSheetId="0">Hoja2!$A$2:$AH$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Task!$A$1:$E$1</definedName>
+    <definedName name="Intino_Usability_Study__respuestas____Respuestas_de_formulario_1" localSheetId="0">Questionary!$A$2:$AH$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -819,7 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -867,6 +867,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -885,11 +886,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF950D56-3666-3441-BE7C-A37A9268B402}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1272,40 +1268,40 @@
     <row r="1" spans="1:34" s="22" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31"/>
       <c r="M1" s="28"/>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="29" t="s">
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31"/>
     </row>
     <row r="2" spans="1:34" s="17" customFormat="1" ht="64" customHeight="1" thickTop="1">
       <c r="A2" s="15" t="s">
@@ -1344,7 +1340,7 @@
       <c r="L2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="15" t="s">
         <v>179</v>
       </c>
       <c r="N2" s="15" t="s">
@@ -1448,7 +1444,7 @@
       <c r="L3" s="19">
         <v>1</v>
       </c>
-      <c r="M3" s="36" t="str">
+      <c r="M3" t="str">
         <f>IF(L3&lt;3,"Novice","Experienced")</f>
         <v>Novice</v>
       </c>
@@ -1552,8 +1548,8 @@
       <c r="L4" s="19">
         <v>1</v>
       </c>
-      <c r="M4" s="36" t="str">
-        <f t="shared" ref="M4:M21" si="1">IF(L4&lt;3,"Novice","Experienced")</f>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M22" si="1">IF(L4&lt;3,"Novice","Experienced")</f>
         <v>Novice</v>
       </c>
       <c r="N4">
@@ -1658,7 +1654,7 @@
       <c r="L5" s="19">
         <v>5</v>
       </c>
-      <c r="M5" s="36" t="str">
+      <c r="M5" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -1704,7 +1700,7 @@
       </c>
       <c r="AA5">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB5">
         <v>3</v>
@@ -1765,7 +1761,7 @@
       <c r="L6" s="19">
         <v>1</v>
       </c>
-      <c r="M6" s="36" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -1871,7 +1867,7 @@
       <c r="L7" s="19">
         <v>3</v>
       </c>
-      <c r="M7" s="36" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -1978,7 +1974,7 @@
       <c r="L8" s="19">
         <v>4</v>
       </c>
-      <c r="M8" s="36" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -2024,7 +2020,7 @@
       </c>
       <c r="AA8">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB8">
         <v>2</v>
@@ -2073,7 +2069,7 @@
       <c r="L9" s="19">
         <v>1</v>
       </c>
-      <c r="M9" s="36" t="str">
+      <c r="M9" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -2119,7 +2115,7 @@
       </c>
       <c r="AA9">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB9">
         <v>3</v>
@@ -2168,7 +2164,7 @@
       <c r="L10" s="19">
         <v>2</v>
       </c>
-      <c r="M10" s="36" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -2274,7 +2270,7 @@
       <c r="L11" s="19">
         <v>5</v>
       </c>
-      <c r="M11" s="36" t="str">
+      <c r="M11" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -2380,7 +2376,7 @@
       <c r="L12" s="20">
         <v>4</v>
       </c>
-      <c r="M12" s="36" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -2478,7 +2474,7 @@
       <c r="L13" s="19">
         <v>1</v>
       </c>
-      <c r="M13" s="36" t="str">
+      <c r="M13" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -2524,7 +2520,7 @@
       </c>
       <c r="AA13">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB13">
         <v>3</v>
@@ -2585,7 +2581,7 @@
       <c r="L14" s="19">
         <v>1</v>
       </c>
-      <c r="M14" s="36" t="str">
+      <c r="M14" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -2691,7 +2687,7 @@
       <c r="L15" s="19">
         <v>5</v>
       </c>
-      <c r="M15" s="36" t="str">
+      <c r="M15" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -2737,7 +2733,7 @@
       </c>
       <c r="AA15">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB15">
         <v>5</v>
@@ -2792,7 +2788,7 @@
       <c r="L16" s="19">
         <v>4</v>
       </c>
-      <c r="M16" s="36" t="str">
+      <c r="M16" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -2899,7 +2895,7 @@
       <c r="L17" s="19">
         <v>5</v>
       </c>
-      <c r="M17" s="36" t="str">
+      <c r="M17" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -3005,7 +3001,7 @@
       <c r="L18" s="19">
         <v>3</v>
       </c>
-      <c r="M18" s="36" t="str">
+      <c r="M18" t="str">
         <f t="shared" si="1"/>
         <v>Experienced</v>
       </c>
@@ -3051,7 +3047,7 @@
       </c>
       <c r="AA18">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB18">
         <v>3</v>
@@ -3109,7 +3105,7 @@
       <c r="L19" s="19">
         <v>1</v>
       </c>
-      <c r="M19" s="36" t="str">
+      <c r="M19" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -3155,7 +3151,7 @@
       </c>
       <c r="AA19">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB19">
         <v>4</v>
@@ -3210,7 +3206,7 @@
       <c r="L20" s="19">
         <v>1</v>
       </c>
-      <c r="M20" s="36" t="str">
+      <c r="M20" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -3256,7 +3252,7 @@
       </c>
       <c r="AA20">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB20">
         <v>4</v>
@@ -3317,7 +3313,7 @@
       <c r="L21" s="19">
         <v>1</v>
       </c>
-      <c r="M21" s="36" t="str">
+      <c r="M21" t="str">
         <f t="shared" si="1"/>
         <v>Novice</v>
       </c>
@@ -3363,7 +3359,7 @@
       </c>
       <c r="AA21">
         <f ca="1">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB21">
         <v>3</v>
@@ -3424,7 +3420,10 @@
       <c r="L22" s="19">
         <v>4</v>
       </c>
-      <c r="M22" s="36"/>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>Experienced</v>
+      </c>
       <c r="N22">
         <v>3</v>
       </c>
@@ -3519,14 +3518,14 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -3544,7 +3543,7 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="23" t="s">
@@ -4084,7 +4083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA8CB26-3099-AF44-80BD-3055C694D6AD}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B36" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
@@ -4100,10 +4099,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
@@ -4122,7 +4121,7 @@
         <v>126</v>
       </c>
       <c r="B3">
-        <f>COUNTA(Hoja2!B3:B22)</f>
+        <f>COUNTA(Questionary!B3:B22)</f>
         <v>20</v>
       </c>
     </row>
@@ -4131,7 +4130,7 @@
         <v>129</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(Hoja2!D3:D22,"Man")</f>
+        <f>COUNTIF(Questionary!D3:D22,"Man")</f>
         <v>18</v>
       </c>
     </row>
@@ -4140,7 +4139,7 @@
         <v>130</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(Hoja2!D3:D22,"Woman")</f>
+        <f>COUNTIF(Questionary!D3:D22,"Woman")</f>
         <v>2</v>
       </c>
     </row>
@@ -4149,11 +4148,11 @@
         <v>132</v>
       </c>
       <c r="B6" s="12">
-        <f>MEDIAN(Hoja2!C3:C22)</f>
+        <f>MEDIAN(Questionary!C3:C22)</f>
         <v>27</v>
       </c>
       <c r="C6" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja2!C3:C22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja2!C3:C22,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Questionary!C3:C22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Questionary!C3:C22,3),3)</f>
         <v>23.75–42.25</v>
       </c>
     </row>
@@ -4162,7 +4161,7 @@
         <v>133</v>
       </c>
       <c r="B7" s="12">
-        <f>MIN(Hoja2!C3:C22)</f>
+        <f>MIN(Questionary!C3:C22)</f>
         <v>20</v>
       </c>
     </row>
@@ -4171,7 +4170,7 @@
         <v>131</v>
       </c>
       <c r="B8" s="12">
-        <f>MAX(Hoja2!C3:C22)</f>
+        <f>MAX(Questionary!C3:C22)</f>
         <v>50</v>
       </c>
     </row>
@@ -4180,11 +4179,11 @@
         <v>134</v>
       </c>
       <c r="B9">
-        <f>MEDIAN(Hoja2!I3:I22)</f>
+        <f>MEDIAN(Questionary!I3:I22)</f>
         <v>5</v>
       </c>
       <c r="C9" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja2!I3:I22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja2!I3:I22,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Questionary!I3:I22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Questionary!I3:I22,3),3)</f>
         <v>2.75–16.25</v>
       </c>
     </row>
@@ -4193,11 +4192,11 @@
         <v>135</v>
       </c>
       <c r="B10">
-        <f>MEDIAN(Hoja2!J3:J22)</f>
+        <f>MEDIAN(Questionary!J3:J22)</f>
         <v>3</v>
       </c>
       <c r="C10" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja2!J3:J22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja2!J3:J22,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Questionary!J3:J22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Questionary!J3:J22,3),3)</f>
         <v>1–5</v>
       </c>
     </row>
@@ -4206,11 +4205,11 @@
         <v>136</v>
       </c>
       <c r="B11">
-        <f>MEDIAN(Hoja2!L3:L22)</f>
+        <f>MEDIAN(Questionary!L3:L22)</f>
         <v>2.5</v>
       </c>
       <c r="C11" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja2!L3:L22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja2!L3:L22,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Questionary!L3:L22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Questionary!L3:L22,3),3)</f>
         <v>1–4</v>
       </c>
     </row>
@@ -4219,7 +4218,7 @@
         <v>137</v>
       </c>
       <c r="B12">
-        <f>COUNTIFS(Hoja2!L3:L22,"&gt;=1",Hoja2!L3:L22,"&lt;=2")</f>
+        <f>COUNTIFS(Questionary!L3:L22,"&gt;=1",Questionary!L3:L22,"&lt;=2")</f>
         <v>10</v>
       </c>
     </row>
@@ -4228,15 +4227,15 @@
         <v>138</v>
       </c>
       <c r="B13">
-        <f>COUNTIFS(Hoja2!L3:L22,"&gt;=3",Hoja2!L3:L22,"&lt;=5")</f>
+        <f>COUNTIFS(Questionary!L3:L22,"&gt;=3",Questionary!L3:L22,"&lt;=5")</f>
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="35"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
@@ -4254,11 +4253,11 @@
         <v>156</v>
       </c>
       <c r="B17">
-        <f>MEDIAN(Hoja1!E2:E21)</f>
+        <f>MEDIAN(Task!E2:E21)</f>
         <v>47</v>
       </c>
       <c r="C17" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja1!E2:E21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja1!E2:E21,3)</f>
+        <f>_xlfn.QUARTILE.INC(Task!E2:E21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Task!E2:E21,3)</f>
         <v>41.75–63.5</v>
       </c>
     </row>
@@ -4267,11 +4266,11 @@
         <v>3</v>
       </c>
       <c r="B18" s="11">
-        <f>MEDIAN(Hoja1!D2:D21)</f>
+        <f>MEDIAN(Task!D2:D21)</f>
         <v>0.7403676210675143</v>
       </c>
       <c r="C18" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja1!D2:D21,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja1!D2:D21,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Task!D2:D21,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Task!D2:D21,3),3)</f>
         <v>0.569–0.84</v>
       </c>
     </row>
@@ -4280,19 +4279,19 @@
         <v>124</v>
       </c>
       <c r="B19" s="11">
-        <f>MEDIAN(Hoja1!F2:F21)</f>
+        <f>MEDIAN(Task!F2:F21)</f>
         <v>1.4864644262958457E-2</v>
       </c>
       <c r="C19" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja1!F2:F21,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja1!F2:F21,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Task!F2:F21,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Task!F2:F21,3),3)</f>
         <v>0.012–0.017</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="35"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
@@ -4310,11 +4309,11 @@
         <v>141</v>
       </c>
       <c r="B23">
-        <f>MEDIAN(Hoja2!X3:X22)</f>
+        <f>MEDIAN(Questionary!X3:X22)</f>
         <v>76.25</v>
       </c>
       <c r="C23" s="26" t="str">
-        <f>TRUNC(_xlfn.QUARTILE.INC(Hoja2!X3:X22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Hoja2!X3:X22,3),3)</f>
+        <f>TRUNC(_xlfn.QUARTILE.INC(Questionary!X3:X22,1),3) &amp; "–" &amp; TRUNC(_xlfn.QUARTILE.INC(Questionary!X3:X22,3),3)</f>
         <v>66.875–85</v>
       </c>
     </row>
@@ -4323,16 +4322,16 @@
         <v>142</v>
       </c>
       <c r="B24" s="27">
-        <f>COUNTIF(Hoja2!X3:X22,"&gt;=70")/COUNTA(Hoja2!X3:X22)</f>
+        <f>COUNTIF(Questionary!X3:X22,"&gt;=70")/COUNTA(Questionary!X3:X22)</f>
         <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
@@ -4350,11 +4349,11 @@
         <v>145</v>
       </c>
       <c r="B28">
-        <f>MEDIAN(Hoja2!Y3:Y22)</f>
+        <f>MEDIAN(Questionary!Y3:Y22)</f>
         <v>4</v>
       </c>
       <c r="C28" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja2!Y3:Y22,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!Y3:Y22,3)</f>
+        <f>_xlfn.QUARTILE.INC(Questionary!Y3:Y22,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!Y3:Y22,3)</f>
         <v>4–5</v>
       </c>
     </row>
@@ -4363,11 +4362,11 @@
         <v>146</v>
       </c>
       <c r="B29">
-        <f>MEDIAN(Hoja2!Z3:Z22)</f>
+        <f>MEDIAN(Questionary!Z3:Z22)</f>
         <v>5</v>
       </c>
       <c r="C29" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja2!Z2:Z21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!Z2:Z21,3)</f>
+        <f>_xlfn.QUARTILE.INC(Questionary!Z2:Z21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!Z2:Z21,3)</f>
         <v>4–5</v>
       </c>
     </row>
@@ -4376,12 +4375,12 @@
         <v>147</v>
       </c>
       <c r="B30">
-        <f ca="1">MEDIAN(Hoja2!AA3:AA22)</f>
+        <f ca="1">MEDIAN(Questionary!AA3:AA22)</f>
         <v>4</v>
       </c>
       <c r="C30" s="26" t="str">
-        <f ca="1">_xlfn.QUARTILE.INC(Hoja2!AA2:AA21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!AA2:AA21,3)</f>
-        <v>4–5</v>
+        <f ca="1">_xlfn.QUARTILE.INC(Questionary!AA2:AA21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!AA2:AA21,3)</f>
+        <v>3–4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4389,11 +4388,11 @@
         <v>148</v>
       </c>
       <c r="B31">
-        <f>MEDIAN(Hoja2!AB3:AB22)</f>
+        <f>MEDIAN(Questionary!AB3:AB22)</f>
         <v>3.5</v>
       </c>
       <c r="C31" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja2!AB2:AB21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!AB2:AB21,3)</f>
+        <f>_xlfn.QUARTILE.INC(Questionary!AB2:AB21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!AB2:AB21,3)</f>
         <v>3–4</v>
       </c>
     </row>
@@ -4402,11 +4401,11 @@
         <v>149</v>
       </c>
       <c r="B32">
-        <f>MEDIAN(Hoja2!AC3:AC22)</f>
+        <f>MEDIAN(Questionary!AC3:AC22)</f>
         <v>4</v>
       </c>
       <c r="C32" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja2!AC2:AC21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!AC2:AC21,3)</f>
+        <f>_xlfn.QUARTILE.INC(Questionary!AC2:AC21,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!AC2:AC21,3)</f>
         <v>3.5–5</v>
       </c>
     </row>
@@ -4415,11 +4414,11 @@
         <v>150</v>
       </c>
       <c r="B33">
-        <f>MEDIAN(Hoja2!AD3:AD23)</f>
+        <f>MEDIAN(Questionary!AD3:AD23)</f>
         <v>4</v>
       </c>
       <c r="C33" s="26" t="str">
-        <f>_xlfn.QUARTILE.INC(Hoja2!AD3:AD22,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Hoja2!AD3:AD22,3)</f>
+        <f>_xlfn.QUARTILE.INC(Questionary!AD3:AD22,1) &amp; "–" &amp; _xlfn.QUARTILE.INC(Questionary!AD3:AD22,3)</f>
         <v>3–5</v>
       </c>
     </row>
@@ -4427,10 +4426,10 @@
       <c r="A35" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B35" s="37" cm="1">
+      <c r="B35" s="29" cm="1">
         <f t="array" ref="B35">_xlfn.LET(
-    _xlpm.grupo, Hoja2!M2:M21,
-    _xlpm.valores, Hoja1!F2:F21,
+    _xlpm.grupo, Questionary!M2:M21,
+    _xlpm.valores, Task!F2:F21,
     _xlpm.x, _xlfn._xlws.FILTER(_xlpm.valores, _xlpm.grupo="Novice"),
     _xlpm.y, _xlfn._xlws.FILTER(_xlpm.valores, _xlpm.grupo="Experienced"),
     _xlpm.nx, ROWS(_xlpm.x),
@@ -4446,10 +4445,10 @@
       <c r="A36" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="B36" s="37" cm="1">
+      <c r="B36" s="29" cm="1">
         <f t="array" ref="B36">_xlfn.LET(
-    _xlpm.grupo, Hoja2!M2:M21,
-    _xlpm.sus, Hoja2!W2:W21,
+    _xlpm.grupo, Questionary!M2:M21,
+    _xlpm.sus, Questionary!W2:W21,
     _xlpm.x, _xlfn._xlws.FILTER(_xlpm.sus, _xlpm.grupo="Novice"),
     _xlpm.y, _xlfn._xlws.FILTER(_xlpm.sus, _xlpm.grupo="Experienced"),
     _xlpm.nx, ROWS(_xlpm.x),

</xml_diff>